<commit_message>
[main]review for tutorial 6
</commit_message>
<xml_diff>
--- a/review_points_EiWahWin.xlsx
+++ b/review_points_EiWahWin.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
   <si>
     <t>Open</t>
     <phoneticPr fontId="1"/>
@@ -217,6 +217,19 @@
   <si>
     <t>Tutorial_03
 login.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Tutorial_06
+1) With no input file and folder name then upload, showing Folder Already Existed.
+2) Use condition for isset both file and folder data
+</t>
+  </si>
+  <si>
+    <t>2)used isset condition for both</t>
+  </si>
+  <si>
+    <t>21/12/2021</t>
   </si>
 </sst>
 </file>
@@ -416,7 +429,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -480,14 +493,23 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -498,6 +520,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -507,38 +541,26 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,7 +599,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51CF917C-11A6-477E-9F8D-8ABC7E2E6625}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{51CF917C-11A6-477E-9F8D-8ABC7E2E6625}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -961,7 +983,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1403,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="I1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="L4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -1439,30 +1461,30 @@
       <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="30" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="32"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="23"/>
       <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="35"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="26"/>
       <c r="V1" s="17" t="s">
         <v>32</v>
       </c>
@@ -1489,30 +1511,30 @@
       <c r="E2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="24" t="s">
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="26"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="29"/>
       <c r="O2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="P2" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
       <c r="V2" s="18" t="s">
         <v>36</v>
       </c>
@@ -1539,28 +1561,28 @@
       <c r="E3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="24" t="s">
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="26"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="29"/>
       <c r="O3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="29"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="36"/>
       <c r="V3" s="18" t="s">
         <v>36</v>
       </c>
@@ -1587,30 +1609,30 @@
       <c r="E4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="24" t="s">
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="26"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="29"/>
       <c r="O4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="29"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="40"/>
       <c r="V4" s="18" t="s">
         <v>42</v>
       </c>
@@ -1635,30 +1657,30 @@
       <c r="E5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="24" t="s">
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="26"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="43"/>
       <c r="O5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="27" t="s">
+      <c r="P5" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="29"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="39"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="40"/>
       <c r="V5" s="18" t="s">
         <v>42</v>
       </c>
@@ -1671,28 +1693,48 @@
     </row>
     <row r="6" spans="1:24" ht="135" customHeight="1">
       <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
+      <c r="B6" s="20">
+        <v>44551</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="39"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="W6" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="X6" s="18"/>
     </row>
     <row r="7" spans="1:24" ht="198.6" customHeight="1">
@@ -1701,28 +1743,33 @@
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="39"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="33"/>
       <c r="O7" s="16"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
       <c r="V7" s="18"/>
       <c r="W7" s="18"/>
       <c r="X7" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="P5:U5"/>
+    <mergeCell ref="P6:U6"/>
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="P1:U1"/>
     <mergeCell ref="F1:H1"/>
@@ -1739,11 +1786,6 @@
     <mergeCell ref="I4:N4"/>
     <mergeCell ref="P4:U4"/>
     <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I5:N5"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="P5:U5"/>
-    <mergeCell ref="P6:U6"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[main]finished for tutorial 8
</commit_message>
<xml_diff>
--- a/review_points_EiWahWin.xlsx
+++ b/review_points_EiWahWin.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Review" sheetId="2" r:id="rId2"/>
     <sheet name="Ref." sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Review!$A$1:$X$18</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
   <si>
     <t>Open</t>
     <phoneticPr fontId="1"/>
@@ -230,6 +233,21 @@
   </si>
   <si>
     <t>21/12/2021</t>
+  </si>
+  <si>
+    <t>Tutorial_07 
+1) Remove unnecessary file</t>
+  </si>
+  <si>
+    <t>Tutorial_06
+index.php</t>
+  </si>
+  <si>
+    <t>Tutorial_07
+index.php</t>
+  </si>
+  <si>
+    <t>1)removed unnecessary file</t>
   </si>
 </sst>
 </file>
@@ -429,7 +447,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -493,6 +511,33 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -511,15 +556,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -544,23 +580,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,7 +620,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{51CF917C-11A6-477E-9F8D-8ABC7E2E6625}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51CF917C-11A6-477E-9F8D-8ABC7E2E6625}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -983,7 +1004,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1425,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="L4" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="X6" sqref="X6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="L1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -1461,30 +1482,30 @@
       <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="21" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="23"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="32"/>
       <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
-      <c r="U1" s="26"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="35"/>
       <c r="V1" s="17" t="s">
         <v>32</v>
       </c>
@@ -1511,30 +1532,30 @@
       <c r="E2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="27" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="29"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="23"/>
       <c r="O2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
       <c r="V2" s="18" t="s">
         <v>36</v>
       </c>
@@ -1561,28 +1582,28 @@
       <c r="E3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="27" t="s">
+      <c r="G3" s="22"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="29"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="23"/>
       <c r="O3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="36"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="42"/>
       <c r="V3" s="18" t="s">
         <v>36</v>
       </c>
@@ -1609,30 +1630,30 @@
       <c r="E4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="27" t="s">
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="29"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="23"/>
       <c r="O4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="38" t="s">
+      <c r="P4" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="40"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="29"/>
       <c r="V4" s="18" t="s">
         <v>42</v>
       </c>
@@ -1644,7 +1665,9 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="135" customHeight="1">
-      <c r="A5" s="19"/>
+      <c r="A5" s="19">
+        <v>4</v>
+      </c>
       <c r="B5" s="20">
         <v>44547</v>
       </c>
@@ -1657,30 +1680,30 @@
       <c r="E5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="41" t="s">
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="43"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="26"/>
       <c r="O5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="38" t="s">
+      <c r="P5" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="40"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="29"/>
       <c r="V5" s="18" t="s">
         <v>42</v>
       </c>
@@ -1692,7 +1715,9 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="135" customHeight="1">
-      <c r="A6" s="19"/>
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
       <c r="B6" s="20">
         <v>44551</v>
       </c>
@@ -1705,30 +1730,30 @@
       <c r="E6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="27" t="s">
+      <c r="F6" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="29"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="23"/>
       <c r="O6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="38" t="s">
+      <c r="P6" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="40"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="29"/>
       <c r="V6" s="18" t="s">
         <v>48</v>
       </c>
@@ -1738,38 +1763,57 @@
       <c r="X6" s="18"/>
     </row>
     <row r="7" spans="1:24" ht="198.6" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
+      <c r="A7" s="19">
+        <v>6</v>
+      </c>
+      <c r="B7" s="20">
+        <v>44552</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="44">
+        <v>44552</v>
+      </c>
+      <c r="W7" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="X7" s="18" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I5:N5"/>
-    <mergeCell ref="I6:N6"/>
-    <mergeCell ref="P5:U5"/>
-    <mergeCell ref="P6:U6"/>
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="P1:U1"/>
     <mergeCell ref="F1:H1"/>
@@ -1786,6 +1830,11 @@
     <mergeCell ref="I4:N4"/>
     <mergeCell ref="P4:U4"/>
     <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="I6:N6"/>
+    <mergeCell ref="P5:U5"/>
+    <mergeCell ref="P6:U6"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[main]finished for review modification
</commit_message>
<xml_diff>
--- a/review_points_EiWahWin.xlsx
+++ b/review_points_EiWahWin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t>Open</t>
     <phoneticPr fontId="1"/>
@@ -248,6 +248,20 @@
   </si>
   <si>
     <t>1)removed unnecessary file</t>
+  </si>
+  <si>
+    <t>Tutorial_08 
+1) Keep old value for already filled fields when validate
+2) Phone Number field not to accept minus value</t>
+  </si>
+  <si>
+    <t>Tutorial_08 
+1) Keeped  old value for already filled fields when validate
+2) changed</t>
+  </si>
+  <si>
+    <t>Tutorial_08
+index.php</t>
   </si>
 </sst>
 </file>
@@ -447,7 +461,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -511,6 +525,9 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -557,6 +574,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -577,11 +597,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1444,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="L1" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="L7" zoomScale="90" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -1482,30 +1505,30 @@
       <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="30" t="s">
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="33"/>
       <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="36"/>
       <c r="V1" s="17" t="s">
         <v>32</v>
       </c>
@@ -1532,30 +1555,30 @@
       <c r="E2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="21" t="s">
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="24"/>
       <c r="O2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="P2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
       <c r="V2" s="18" t="s">
         <v>36</v>
       </c>
@@ -1582,28 +1605,28 @@
       <c r="E3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="21" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
       <c r="O3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="42"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="44"/>
       <c r="V3" s="18" t="s">
         <v>36</v>
       </c>
@@ -1630,30 +1653,30 @@
       <c r="E4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="21" t="s">
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
       <c r="O4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="27" t="s">
+      <c r="P4" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="30"/>
       <c r="V4" s="18" t="s">
         <v>42</v>
       </c>
@@ -1680,30 +1703,30 @@
       <c r="E5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="24" t="s">
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="27"/>
       <c r="O5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="27" t="s">
+      <c r="P5" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="30"/>
       <c r="V5" s="18" t="s">
         <v>42</v>
       </c>
@@ -1730,30 +1753,30 @@
       <c r="E6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="21" t="s">
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="24"/>
       <c r="O6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="27" t="s">
+      <c r="P6" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="30"/>
       <c r="V6" s="18" t="s">
         <v>48</v>
       </c>
@@ -1778,31 +1801,31 @@
       <c r="E7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="21" t="s">
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="39"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="41"/>
       <c r="O7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="P7" s="37" t="s">
+      <c r="P7" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="44">
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
+      <c r="V7" s="21">
         <v>44552</v>
       </c>
       <c r="W7" s="18" t="s">
@@ -1812,8 +1835,63 @@
         <v>38</v>
       </c>
     </row>
+    <row r="8" spans="1:24" ht="123.75" customHeight="1">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="45">
+        <v>44552</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
+      <c r="S8" s="47"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="45">
+        <v>44552</v>
+      </c>
+      <c r="W8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="X8" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="108.75" customHeight="1"/>
+    <row r="10" spans="1:24" ht="108.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="24">
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:N8"/>
+    <mergeCell ref="P8:U8"/>
     <mergeCell ref="I1:N1"/>
     <mergeCell ref="P1:U1"/>
     <mergeCell ref="F1:H1"/>

</xml_diff>